<commit_message>
Added 2 missing values
</commit_message>
<xml_diff>
--- a/analysis/model_evaluation/random_500_comments.xlsx
+++ b/analysis/model_evaluation/random_500_comments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bradley/Desktop/SMT203/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weikh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0A4312FF-0089-C44F-9166-40CF7CBB2A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62090C12-D4D4-4901-BEC8-3387232CFD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="random_500_comments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3014" uniqueCount="1015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3016" uniqueCount="1015">
   <si>
     <t>username</t>
   </si>
@@ -3401,7 +3401,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -4239,19 +4239,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E502" sqref="E502"/>
+    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="E178" sqref="E178"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="186.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>641425</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1129047</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>635246</v>
       </c>
@@ -4460,7 +4460,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="186" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>551725</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>868356</v>
       </c>
@@ -4566,7 +4566,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>838262</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>894601</v>
       </c>
@@ -4672,7 +4672,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>840986</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>822159</v>
       </c>
@@ -4778,7 +4778,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>868577</v>
       </c>
@@ -4831,7 +4831,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>546893</v>
       </c>
@@ -4884,7 +4884,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>88793</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>995905</v>
       </c>
@@ -4990,7 +4990,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>668435</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>297046</v>
       </c>
@@ -5096,7 +5096,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>847747</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>201295</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>418704</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>603150</v>
       </c>
@@ -5308,7 +5308,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>881875</v>
       </c>
@@ -5361,7 +5361,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>993319</v>
       </c>
@@ -5414,7 +5414,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>294732</v>
       </c>
@@ -5467,7 +5467,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>114439</v>
       </c>
@@ -5520,7 +5520,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>620029</v>
       </c>
@@ -5573,7 +5573,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1019983</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>287889</v>
       </c>
@@ -5679,7 +5679,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>695420</v>
       </c>
@@ -5732,7 +5732,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>678007</v>
       </c>
@@ -5785,7 +5785,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>430817</v>
       </c>
@@ -5838,7 +5838,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>388791</v>
       </c>
@@ -5891,7 +5891,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>876996</v>
       </c>
@@ -5944,7 +5944,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>614993</v>
       </c>
@@ -5997,7 +5997,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>289995</v>
       </c>
@@ -6050,7 +6050,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>916688</v>
       </c>
@@ -6103,7 +6103,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>550292</v>
       </c>
@@ -6156,7 +6156,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>266339</v>
       </c>
@@ -6209,7 +6209,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>634113</v>
       </c>
@@ -6262,7 +6262,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>504665</v>
       </c>
@@ -6315,7 +6315,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>463951</v>
       </c>
@@ -6368,7 +6368,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>999405</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>554358</v>
       </c>
@@ -6474,7 +6474,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>551970</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>567094</v>
       </c>
@@ -6580,7 +6580,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>558341</v>
       </c>
@@ -6633,7 +6633,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>656499</v>
       </c>
@@ -6686,7 +6686,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>937461</v>
       </c>
@@ -6739,7 +6739,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>899374</v>
       </c>
@@ -6792,7 +6792,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>607567</v>
       </c>
@@ -6845,7 +6845,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>622644</v>
       </c>
@@ -6898,7 +6898,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" ht="93" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>844792</v>
       </c>
@@ -6951,7 +6951,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>609808</v>
       </c>
@@ -7004,7 +7004,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>659347</v>
       </c>
@@ -7057,7 +7057,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>1092208</v>
       </c>
@@ -7110,7 +7110,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>514387</v>
       </c>
@@ -7163,7 +7163,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>293026</v>
       </c>
@@ -7216,7 +7216,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>81898</v>
       </c>
@@ -7269,7 +7269,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>621698</v>
       </c>
@@ -7322,7 +7322,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>594644</v>
       </c>
@@ -7375,7 +7375,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>801567</v>
       </c>
@@ -7428,7 +7428,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>369008</v>
       </c>
@@ -7481,7 +7481,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>540406</v>
       </c>
@@ -7534,7 +7534,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>387447</v>
       </c>
@@ -7587,7 +7587,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>1115858</v>
       </c>
@@ -7640,7 +7640,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>724934</v>
       </c>
@@ -7693,7 +7693,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>1066804</v>
       </c>
@@ -7746,7 +7746,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>868346</v>
       </c>
@@ -7799,7 +7799,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>758883</v>
       </c>
@@ -7852,7 +7852,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>622157</v>
       </c>
@@ -7905,7 +7905,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>778751</v>
       </c>
@@ -7958,7 +7958,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>602227</v>
       </c>
@@ -7971,6 +7971,9 @@
       <c r="D71" t="s">
         <v>187</v>
       </c>
+      <c r="E71" t="s">
+        <v>27</v>
+      </c>
       <c r="F71">
         <v>0</v>
       </c>
@@ -8008,7 +8011,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>1099596</v>
       </c>
@@ -8061,7 +8064,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>74180</v>
       </c>
@@ -8114,7 +8117,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>863993</v>
       </c>
@@ -8167,7 +8170,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1077437</v>
       </c>
@@ -8220,7 +8223,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17" ht="232.5" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>783954</v>
       </c>
@@ -8273,7 +8276,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>757947</v>
       </c>
@@ -8326,7 +8329,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>1115140</v>
       </c>
@@ -8379,7 +8382,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>710915</v>
       </c>
@@ -8432,7 +8435,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>659358</v>
       </c>
@@ -8485,7 +8488,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>875881</v>
       </c>
@@ -8538,7 +8541,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>713632</v>
       </c>
@@ -8591,7 +8594,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>729429</v>
       </c>
@@ -8644,7 +8647,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>993357</v>
       </c>
@@ -8697,7 +8700,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>750177</v>
       </c>
@@ -8750,7 +8753,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>728287</v>
       </c>
@@ -8803,7 +8806,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>675644</v>
       </c>
@@ -8856,7 +8859,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>1056422</v>
       </c>
@@ -8909,7 +8912,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>1086693</v>
       </c>
@@ -8962,7 +8965,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>105669</v>
       </c>
@@ -9015,7 +9018,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:17" ht="217" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>558584</v>
       </c>
@@ -9068,7 +9071,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>476072</v>
       </c>
@@ -9121,7 +9124,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:17" ht="62" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>543530</v>
       </c>
@@ -9174,7 +9177,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:17" ht="62" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>594615</v>
       </c>
@@ -9227,7 +9230,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>863236</v>
       </c>
@@ -9280,7 +9283,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>982253</v>
       </c>
@@ -9333,7 +9336,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:17" ht="124" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>775587</v>
       </c>
@@ -9386,7 +9389,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>105346</v>
       </c>
@@ -9439,7 +9442,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>407536</v>
       </c>
@@ -9492,7 +9495,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>705118</v>
       </c>
@@ -9545,7 +9548,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>1098997</v>
       </c>
@@ -9598,7 +9601,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:17" ht="93" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>753303</v>
       </c>
@@ -9651,7 +9654,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>604661</v>
       </c>
@@ -9704,7 +9707,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>725391</v>
       </c>
@@ -9757,7 +9760,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>579044</v>
       </c>
@@ -9810,7 +9813,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>725743</v>
       </c>
@@ -9863,7 +9866,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>1149</v>
       </c>
@@ -9916,7 +9919,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>686092</v>
       </c>
@@ -9969,7 +9972,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>1007777</v>
       </c>
@@ -10022,7 +10025,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>101965</v>
       </c>
@@ -10075,7 +10078,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>1109097</v>
       </c>
@@ -10128,7 +10131,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>1138915</v>
       </c>
@@ -10181,7 +10184,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>995252</v>
       </c>
@@ -10234,7 +10237,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>539574</v>
       </c>
@@ -10287,7 +10290,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>1014802</v>
       </c>
@@ -10340,7 +10343,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>1070170</v>
       </c>
@@ -10393,7 +10396,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>713494</v>
       </c>
@@ -10446,7 +10449,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>658201</v>
       </c>
@@ -10499,7 +10502,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>594965</v>
       </c>
@@ -10552,7 +10555,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:17" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>689560</v>
       </c>
@@ -10605,7 +10608,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>1142569</v>
       </c>
@@ -10658,7 +10661,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>286161</v>
       </c>
@@ -10711,7 +10714,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>999414</v>
       </c>
@@ -10764,7 +10767,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>919534</v>
       </c>
@@ -10817,7 +10820,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>1032802</v>
       </c>
@@ -10870,7 +10873,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>1018738</v>
       </c>
@@ -10923,7 +10926,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>677644</v>
       </c>
@@ -10976,7 +10979,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>109381</v>
       </c>
@@ -11029,7 +11032,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>517329</v>
       </c>
@@ -11082,7 +11085,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>770194</v>
       </c>
@@ -11135,7 +11138,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>707962</v>
       </c>
@@ -11188,7 +11191,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>927382</v>
       </c>
@@ -11241,7 +11244,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>1105541</v>
       </c>
@@ -11294,7 +11297,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>215906</v>
       </c>
@@ -11347,7 +11350,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>375947</v>
       </c>
@@ -11400,7 +11403,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>517492</v>
       </c>
@@ -11453,7 +11456,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>101545</v>
       </c>
@@ -11506,7 +11509,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>855186</v>
       </c>
@@ -11559,7 +11562,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>731282</v>
       </c>
@@ -11612,7 +11615,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>814427</v>
       </c>
@@ -11665,7 +11668,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>718622</v>
       </c>
@@ -11718,7 +11721,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>679746</v>
       </c>
@@ -11771,7 +11774,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>30038</v>
       </c>
@@ -11824,7 +11827,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>1153289</v>
       </c>
@@ -11877,7 +11880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>770064</v>
       </c>
@@ -11930,7 +11933,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>779300</v>
       </c>
@@ -11983,7 +11986,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>280753</v>
       </c>
@@ -12036,7 +12039,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>628233</v>
       </c>
@@ -12089,7 +12092,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>732064</v>
       </c>
@@ -12142,7 +12145,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>109241</v>
       </c>
@@ -12195,7 +12198,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>631551</v>
       </c>
@@ -12248,7 +12251,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>265976</v>
       </c>
@@ -12301,7 +12304,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>1076015</v>
       </c>
@@ -12354,7 +12357,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>625522</v>
       </c>
@@ -12407,7 +12410,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>1129160</v>
       </c>
@@ -12460,7 +12463,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>613144</v>
       </c>
@@ -12513,7 +12516,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>801943</v>
       </c>
@@ -12566,7 +12569,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>915773</v>
       </c>
@@ -12619,7 +12622,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>1039290</v>
       </c>
@@ -12672,7 +12675,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>868258</v>
       </c>
@@ -12725,7 +12728,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>281433</v>
       </c>
@@ -12778,7 +12781,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:17" ht="155" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>770825</v>
       </c>
@@ -12831,7 +12834,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>652131</v>
       </c>
@@ -12884,7 +12887,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>47549</v>
       </c>
@@ -12937,7 +12940,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>101526</v>
       </c>
@@ -12990,7 +12993,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>869576</v>
       </c>
@@ -13043,7 +13046,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>953406</v>
       </c>
@@ -13096,7 +13099,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>374432</v>
       </c>
@@ -13149,7 +13152,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>865326</v>
       </c>
@@ -13202,7 +13205,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>101965</v>
       </c>
@@ -13255,7 +13258,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>821747</v>
       </c>
@@ -13308,7 +13311,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>282228</v>
       </c>
@@ -13361,7 +13364,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>954212</v>
       </c>
@@ -13414,7 +13417,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>276638</v>
       </c>
@@ -13467,7 +13470,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>1068274</v>
       </c>
@@ -13520,7 +13523,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>900677</v>
       </c>
@@ -13573,7 +13576,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>592261</v>
       </c>
@@ -13586,6 +13589,9 @@
       <c r="D177" t="s">
         <v>395</v>
       </c>
+      <c r="E177" t="s">
+        <v>18</v>
+      </c>
       <c r="F177">
         <v>0</v>
       </c>
@@ -13623,7 +13629,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>521766</v>
       </c>
@@ -13676,7 +13682,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>83652</v>
       </c>
@@ -13729,7 +13735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>724677</v>
       </c>
@@ -13782,7 +13788,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>280597</v>
       </c>
@@ -13835,7 +13841,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>573993</v>
       </c>
@@ -13888,7 +13894,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>704782</v>
       </c>
@@ -13941,7 +13947,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>889228</v>
       </c>
@@ -13994,7 +14000,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="185" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>991218</v>
       </c>
@@ -14047,7 +14053,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>699409</v>
       </c>
@@ -14100,7 +14106,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:17" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>589929</v>
       </c>
@@ -14153,7 +14159,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>388195</v>
       </c>
@@ -14206,7 +14212,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>266315</v>
       </c>
@@ -14259,7 +14265,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="190" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>292675</v>
       </c>
@@ -14312,7 +14318,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="191" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>222938</v>
       </c>
@@ -14365,7 +14371,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="192" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>1096243</v>
       </c>
@@ -14418,7 +14424,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>673180</v>
       </c>
@@ -14471,7 +14477,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="194" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>901744</v>
       </c>
@@ -14524,7 +14530,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A195">
         <v>857480</v>
       </c>
@@ -14577,7 +14583,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A196">
         <v>512621</v>
       </c>
@@ -14630,7 +14636,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A197">
         <v>835690</v>
       </c>
@@ -14683,7 +14689,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A198">
         <v>661989</v>
       </c>
@@ -14736,7 +14742,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>610241</v>
       </c>
@@ -14789,7 +14795,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A200">
         <v>582465</v>
       </c>
@@ -14842,7 +14848,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A201">
         <v>1127935</v>
       </c>
@@ -14895,7 +14901,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A202">
         <v>1115132</v>
       </c>
@@ -14948,7 +14954,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="203" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A203">
         <v>226203</v>
       </c>
@@ -15001,7 +15007,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A204">
         <v>372771</v>
       </c>
@@ -15054,7 +15060,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A205">
         <v>285950</v>
       </c>
@@ -15107,7 +15113,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A206">
         <v>293691</v>
       </c>
@@ -15160,7 +15166,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A207">
         <v>457067</v>
       </c>
@@ -15213,7 +15219,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A208">
         <v>898669</v>
       </c>
@@ -15266,7 +15272,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A209">
         <v>882780</v>
       </c>
@@ -15319,7 +15325,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A210">
         <v>865590</v>
       </c>
@@ -15372,7 +15378,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A211">
         <v>836653</v>
       </c>
@@ -15425,7 +15431,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>504380</v>
       </c>
@@ -15478,7 +15484,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:17" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A213">
         <v>630657</v>
       </c>
@@ -15531,7 +15537,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A214">
         <v>652876</v>
       </c>
@@ -15584,7 +15590,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A215">
         <v>818692</v>
       </c>
@@ -15637,7 +15643,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>281558</v>
       </c>
@@ -15690,7 +15696,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>1134636</v>
       </c>
@@ -15743,7 +15749,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A218">
         <v>735384</v>
       </c>
@@ -15796,7 +15802,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A219">
         <v>864688</v>
       </c>
@@ -15849,7 +15855,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>550740</v>
       </c>
@@ -15902,7 +15908,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="221" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>1038973</v>
       </c>
@@ -15955,7 +15961,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A222">
         <v>300808</v>
       </c>
@@ -16008,7 +16014,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A223">
         <v>650402</v>
       </c>
@@ -16061,7 +16067,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>174181</v>
       </c>
@@ -16114,7 +16120,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>89359</v>
       </c>
@@ -16167,7 +16173,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="226" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A226">
         <v>803395</v>
       </c>
@@ -16220,7 +16226,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="227" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A227">
         <v>1030187</v>
       </c>
@@ -16273,7 +16279,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="228" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A228">
         <v>829054</v>
       </c>
@@ -16326,7 +16332,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="229" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A229">
         <v>296775</v>
       </c>
@@ -16379,7 +16385,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="230" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A230">
         <v>32012</v>
       </c>
@@ -16432,7 +16438,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="231" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A231">
         <v>713139</v>
       </c>
@@ -16485,7 +16491,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="232" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A232">
         <v>1078437</v>
       </c>
@@ -16538,7 +16544,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="233" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A233">
         <v>378071</v>
       </c>
@@ -16591,7 +16597,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="234" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:17" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A234">
         <v>903172</v>
       </c>
@@ -16644,7 +16650,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="235" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A235">
         <v>608180</v>
       </c>
@@ -16697,7 +16703,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="236" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A236">
         <v>698879</v>
       </c>
@@ -16750,7 +16756,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="237" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A237">
         <v>114512</v>
       </c>
@@ -16803,7 +16809,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="238" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A238">
         <v>363916</v>
       </c>
@@ -16856,7 +16862,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="239" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A239">
         <v>342700</v>
       </c>
@@ -16909,7 +16915,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="240" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A240">
         <v>1026000</v>
       </c>
@@ -16962,7 +16968,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="241" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A241">
         <v>564497</v>
       </c>
@@ -17015,7 +17021,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A242">
         <v>1066008</v>
       </c>
@@ -17068,7 +17074,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="243" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A243">
         <v>509105</v>
       </c>
@@ -17121,7 +17127,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="244" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A244">
         <v>39016</v>
       </c>
@@ -17174,7 +17180,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="245" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A245">
         <v>869013</v>
       </c>
@@ -17227,7 +17233,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="246" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A246">
         <v>372064</v>
       </c>
@@ -17280,7 +17286,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="247" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A247">
         <v>826522</v>
       </c>
@@ -17333,7 +17339,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="248" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A248">
         <v>243815</v>
       </c>
@@ -17386,7 +17392,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="249" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A249">
         <v>638179</v>
       </c>
@@ -17439,7 +17445,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="250" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A250">
         <v>1148286</v>
       </c>
@@ -17492,7 +17498,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="251" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A251">
         <v>62178</v>
       </c>
@@ -17545,7 +17551,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="252" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A252">
         <v>14087</v>
       </c>
@@ -17598,7 +17604,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="253" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A253">
         <v>1100219</v>
       </c>
@@ -17651,7 +17657,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="254" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A254">
         <v>92810</v>
       </c>
@@ -17704,7 +17710,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="255" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A255">
         <v>865319</v>
       </c>
@@ -17757,7 +17763,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="256" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A256">
         <v>726774</v>
       </c>
@@ -17810,7 +17816,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A257">
         <v>470098</v>
       </c>
@@ -17863,7 +17869,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A258">
         <v>1140760</v>
       </c>
@@ -17916,7 +17922,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="259" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A259">
         <v>218489</v>
       </c>
@@ -17969,7 +17975,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A260">
         <v>712717</v>
       </c>
@@ -18022,7 +18028,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="261" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A261">
         <v>27839</v>
       </c>
@@ -18075,7 +18081,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="262" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A262">
         <v>117150</v>
       </c>
@@ -18128,7 +18134,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="263" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A263">
         <v>991959</v>
       </c>
@@ -18181,7 +18187,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="264" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A264">
         <v>371632</v>
       </c>
@@ -18234,7 +18240,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="265" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A265">
         <v>954414</v>
       </c>
@@ -18287,7 +18293,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="266" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A266">
         <v>675432</v>
       </c>
@@ -18340,7 +18346,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="267" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A267">
         <v>53745</v>
       </c>
@@ -18393,7 +18399,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="268" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A268">
         <v>1136553</v>
       </c>
@@ -18446,7 +18452,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="269" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A269">
         <v>685960</v>
       </c>
@@ -18499,7 +18505,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="270" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A270">
         <v>491835</v>
       </c>
@@ -18552,7 +18558,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="271" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A271">
         <v>17797</v>
       </c>
@@ -18605,7 +18611,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="272" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A272">
         <v>18956</v>
       </c>
@@ -18658,7 +18664,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="273" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A273">
         <v>290008</v>
       </c>
@@ -18711,7 +18717,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="274" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A274">
         <v>429509</v>
       </c>
@@ -18764,7 +18770,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="275" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A275">
         <v>137957</v>
       </c>
@@ -18817,7 +18823,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="276" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A276">
         <v>552587</v>
       </c>
@@ -18870,7 +18876,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="277" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A277">
         <v>370852</v>
       </c>
@@ -18923,7 +18929,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="278" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A278">
         <v>637865</v>
       </c>
@@ -18976,7 +18982,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="279" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A279">
         <v>983506</v>
       </c>
@@ -19029,7 +19035,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="280" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A280">
         <v>1101192</v>
       </c>
@@ -19082,7 +19088,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="281" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A281">
         <v>645380</v>
       </c>
@@ -19135,7 +19141,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="282" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A282">
         <v>25044</v>
       </c>
@@ -19188,7 +19194,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="283" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A283">
         <v>298826</v>
       </c>
@@ -19241,7 +19247,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="284" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A284">
         <v>377935</v>
       </c>
@@ -19294,7 +19300,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="285" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A285">
         <v>759833</v>
       </c>
@@ -19347,7 +19353,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="286" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A286">
         <v>1134843</v>
       </c>
@@ -19400,7 +19406,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="287" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A287">
         <v>500352</v>
       </c>
@@ -19453,7 +19459,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="288" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A288">
         <v>409165</v>
       </c>
@@ -19506,7 +19512,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="289" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A289">
         <v>925926</v>
       </c>
@@ -19559,7 +19565,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="290" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A290">
         <v>374899</v>
       </c>
@@ -19612,7 +19618,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="291" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A291">
         <v>526173</v>
       </c>
@@ -19665,7 +19671,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="292" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A292">
         <v>343515</v>
       </c>
@@ -19718,7 +19724,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="293" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A293">
         <v>374740</v>
       </c>
@@ -19771,7 +19777,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="294" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A294">
         <v>399490</v>
       </c>
@@ -19824,7 +19830,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="295" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A295">
         <v>813305</v>
       </c>
@@ -19877,7 +19883,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="296" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A296">
         <v>365161</v>
       </c>
@@ -19930,7 +19936,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="297" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A297">
         <v>1113120</v>
       </c>
@@ -19983,7 +19989,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="298" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A298">
         <v>1082121</v>
       </c>
@@ -20036,7 +20042,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="299" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:17" ht="217" x14ac:dyDescent="0.35">
       <c r="A299">
         <v>793463</v>
       </c>
@@ -20089,7 +20095,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="300" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A300">
         <v>165724</v>
       </c>
@@ -20142,7 +20148,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="301" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A301">
         <v>31831</v>
       </c>
@@ -20195,7 +20201,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="302" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A302">
         <v>495323</v>
       </c>
@@ -20248,7 +20254,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="303" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A303">
         <v>547401</v>
       </c>
@@ -20301,7 +20307,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="304" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A304">
         <v>120641</v>
       </c>
@@ -20354,7 +20360,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="305" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A305">
         <v>546130</v>
       </c>
@@ -20407,7 +20413,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="306" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A306">
         <v>595251</v>
       </c>
@@ -20460,7 +20466,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="307" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A307">
         <v>1137503</v>
       </c>
@@ -20513,7 +20519,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="308" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A308">
         <v>117394</v>
       </c>
@@ -20566,7 +20572,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="309" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A309">
         <v>960706</v>
       </c>
@@ -20619,7 +20625,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="310" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A310">
         <v>973290</v>
       </c>
@@ -20672,7 +20678,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="311" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A311">
         <v>95506</v>
       </c>
@@ -20725,7 +20731,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="312" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A312">
         <v>853463</v>
       </c>
@@ -20778,7 +20784,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="313" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A313">
         <v>223968</v>
       </c>
@@ -20831,7 +20837,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="314" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A314">
         <v>585820</v>
       </c>
@@ -20884,7 +20890,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="315" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A315">
         <v>1090033</v>
       </c>
@@ -20937,7 +20943,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="316" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A316">
         <v>1131820</v>
       </c>
@@ -20990,7 +20996,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="317" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A317">
         <v>368669</v>
       </c>
@@ -21043,7 +21049,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="318" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A318">
         <v>639747</v>
       </c>
@@ -21096,7 +21102,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="319" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A319">
         <v>140351</v>
       </c>
@@ -21149,7 +21155,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="320" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A320">
         <v>250484</v>
       </c>
@@ -21202,7 +21208,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="321" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A321">
         <v>124118</v>
       </c>
@@ -21255,7 +21261,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="322" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A322">
         <v>188657</v>
       </c>
@@ -21308,7 +21314,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="323" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A323">
         <v>664565</v>
       </c>
@@ -21361,7 +21367,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="324" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A324">
         <v>170188</v>
       </c>
@@ -21414,7 +21420,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="325" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A325">
         <v>898021</v>
       </c>
@@ -21467,7 +21473,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="326" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A326">
         <v>977939</v>
       </c>
@@ -21520,7 +21526,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="327" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A327">
         <v>454710</v>
       </c>
@@ -21573,7 +21579,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="328" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A328">
         <v>864530</v>
       </c>
@@ -21626,7 +21632,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="329" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A329">
         <v>309641</v>
       </c>
@@ -21679,7 +21685,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="330" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A330">
         <v>178413</v>
       </c>
@@ -21732,7 +21738,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="331" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A331">
         <v>433476</v>
       </c>
@@ -21785,7 +21791,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="332" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A332">
         <v>744391</v>
       </c>
@@ -21838,7 +21844,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="333" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A333">
         <v>74381</v>
       </c>
@@ -21891,7 +21897,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="334" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A334">
         <v>373418</v>
       </c>
@@ -21944,7 +21950,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="335" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A335">
         <v>444226</v>
       </c>
@@ -21997,7 +22003,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="336" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A336">
         <v>842802</v>
       </c>
@@ -22050,7 +22056,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="337" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A337">
         <v>453056</v>
       </c>
@@ -22103,7 +22109,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="338" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A338">
         <v>335876</v>
       </c>
@@ -22156,7 +22162,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="339" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A339">
         <v>798475</v>
       </c>
@@ -22209,7 +22215,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="340" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A340">
         <v>805866</v>
       </c>
@@ -22262,7 +22268,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="341" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A341">
         <v>144170</v>
       </c>
@@ -22315,7 +22321,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="342" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A342">
         <v>295940</v>
       </c>
@@ -22368,7 +22374,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="343" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A343">
         <v>121391</v>
       </c>
@@ -22421,7 +22427,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="344" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A344">
         <v>109056</v>
       </c>
@@ -22474,7 +22480,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="345" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A345">
         <v>135942</v>
       </c>
@@ -22527,7 +22533,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="346" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A346">
         <v>91622</v>
       </c>
@@ -22580,7 +22586,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="347" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A347">
         <v>216536</v>
       </c>
@@ -22633,7 +22639,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="348" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A348">
         <v>786739</v>
       </c>
@@ -22686,7 +22692,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="349" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A349">
         <v>866057</v>
       </c>
@@ -22739,7 +22745,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="350" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A350">
         <v>1063869</v>
       </c>
@@ -22792,7 +22798,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="351" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A351">
         <v>181006</v>
       </c>
@@ -22845,7 +22851,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="352" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A352">
         <v>126629</v>
       </c>
@@ -22898,7 +22904,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="353" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A353">
         <v>437360</v>
       </c>
@@ -22951,7 +22957,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="354" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A354">
         <v>202834</v>
       </c>
@@ -23004,7 +23010,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="355" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A355">
         <v>609526</v>
       </c>
@@ -23057,7 +23063,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="356" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A356">
         <v>1026780</v>
       </c>
@@ -23110,7 +23116,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="357" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A357">
         <v>271533</v>
       </c>
@@ -23163,7 +23169,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="358" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A358">
         <v>571544</v>
       </c>
@@ -23216,7 +23222,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="359" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A359">
         <v>971985</v>
       </c>
@@ -23269,7 +23275,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="360" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A360">
         <v>1145739</v>
       </c>
@@ -23322,7 +23328,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="361" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A361">
         <v>411425</v>
       </c>
@@ -23375,7 +23381,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="362" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A362">
         <v>1029962</v>
       </c>
@@ -23428,7 +23434,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="363" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A363">
         <v>170032</v>
       </c>
@@ -23481,7 +23487,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="364" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A364">
         <v>829031</v>
       </c>
@@ -23534,7 +23540,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="365" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A365">
         <v>176971</v>
       </c>
@@ -23587,7 +23593,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="366" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A366">
         <v>893026</v>
       </c>
@@ -23640,7 +23646,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="367" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A367">
         <v>374467</v>
       </c>
@@ -23693,7 +23699,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="368" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A368">
         <v>53698</v>
       </c>
@@ -23746,7 +23752,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="369" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A369">
         <v>443551</v>
       </c>
@@ -23799,7 +23805,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="370" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A370">
         <v>15620</v>
       </c>
@@ -23852,7 +23858,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="371" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:17" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A371">
         <v>770447</v>
       </c>
@@ -23905,7 +23911,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="372" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A372">
         <v>997723</v>
       </c>
@@ -23958,7 +23964,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="373" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A373">
         <v>530166</v>
       </c>
@@ -24011,7 +24017,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="374" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A374">
         <v>1054953</v>
       </c>
@@ -24064,7 +24070,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="375" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A375">
         <v>408181</v>
       </c>
@@ -24117,7 +24123,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="376" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A376">
         <v>1030284</v>
       </c>
@@ -24170,7 +24176,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="377" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A377">
         <v>476823</v>
       </c>
@@ -24223,7 +24229,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="378" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A378">
         <v>1055635</v>
       </c>
@@ -24276,7 +24282,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="379" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A379">
         <v>292483</v>
       </c>
@@ -24329,7 +24335,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="380" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A380">
         <v>994340</v>
       </c>
@@ -24382,7 +24388,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="381" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A381">
         <v>1011786</v>
       </c>
@@ -24435,7 +24441,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="382" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:17" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A382">
         <v>508688</v>
       </c>
@@ -24488,7 +24494,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="383" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A383">
         <v>661378</v>
       </c>
@@ -24541,7 +24547,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="384" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A384">
         <v>806669</v>
       </c>
@@ -24594,7 +24600,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="385" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A385">
         <v>473342</v>
       </c>
@@ -24647,7 +24653,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="386" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A386">
         <v>764071</v>
       </c>
@@ -24700,7 +24706,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="387" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A387">
         <v>22377</v>
       </c>
@@ -24753,7 +24759,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="388" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A388">
         <v>419402</v>
       </c>
@@ -24806,7 +24812,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="389" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A389">
         <v>799241</v>
       </c>
@@ -24859,7 +24865,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="390" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A390">
         <v>357810</v>
       </c>
@@ -24912,7 +24918,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="391" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A391">
         <v>979040</v>
       </c>
@@ -24965,7 +24971,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="392" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A392">
         <v>231470</v>
       </c>
@@ -25018,7 +25024,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="393" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A393">
         <v>471330</v>
       </c>
@@ -25071,7 +25077,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="394" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A394">
         <v>129151</v>
       </c>
@@ -25124,7 +25130,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="395" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A395">
         <v>303691</v>
       </c>
@@ -25177,7 +25183,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="396" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A396">
         <v>846151</v>
       </c>
@@ -25230,7 +25236,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="397" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A397">
         <v>67597</v>
       </c>
@@ -25283,7 +25289,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="398" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A398">
         <v>788675</v>
       </c>
@@ -25336,7 +25342,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="399" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A399">
         <v>494761</v>
       </c>
@@ -25389,7 +25395,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="400" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A400">
         <v>900563</v>
       </c>
@@ -25442,7 +25448,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="401" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A401">
         <v>350625</v>
       </c>
@@ -25495,7 +25501,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="402" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A402">
         <v>173715</v>
       </c>
@@ -25548,7 +25554,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="403" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A403">
         <v>1102942</v>
       </c>
@@ -25601,7 +25607,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="404" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A404">
         <v>165624</v>
       </c>
@@ -25654,7 +25660,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="405" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A405">
         <v>221515</v>
       </c>
@@ -25707,7 +25713,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="406" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A406">
         <v>1007692</v>
       </c>
@@ -25760,7 +25766,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="407" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A407">
         <v>687752</v>
       </c>
@@ -25813,7 +25819,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="408" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A408">
         <v>653227</v>
       </c>
@@ -25866,7 +25872,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="409" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A409">
         <v>500860</v>
       </c>
@@ -25919,7 +25925,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="410" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A410">
         <v>8982</v>
       </c>
@@ -25972,7 +25978,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="411" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A411">
         <v>1027643</v>
       </c>
@@ -26025,7 +26031,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="412" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:17" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A412">
         <v>724552</v>
       </c>
@@ -26078,7 +26084,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="413" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A413">
         <v>763961</v>
       </c>
@@ -26131,7 +26137,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="414" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A414">
         <v>589462</v>
       </c>
@@ -26184,7 +26190,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="415" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A415">
         <v>535577</v>
       </c>
@@ -26237,7 +26243,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="416" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A416">
         <v>823713</v>
       </c>
@@ -26290,7 +26296,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="417" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:17" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A417">
         <v>761828</v>
       </c>
@@ -26343,7 +26349,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="418" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A418">
         <v>671439</v>
       </c>
@@ -26396,7 +26402,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="419" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A419">
         <v>320814</v>
       </c>
@@ -26449,7 +26455,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="420" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A420">
         <v>1133631</v>
       </c>
@@ -26502,7 +26508,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="421" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A421">
         <v>287185</v>
       </c>
@@ -26555,7 +26561,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="422" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A422">
         <v>206280</v>
       </c>
@@ -26608,7 +26614,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="423" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A423">
         <v>269805</v>
       </c>
@@ -26661,7 +26667,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="424" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A424">
         <v>1097527</v>
       </c>
@@ -26714,7 +26720,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="425" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A425">
         <v>823310</v>
       </c>
@@ -26767,7 +26773,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="426" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A426">
         <v>488560</v>
       </c>
@@ -26820,7 +26826,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="427" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A427">
         <v>289315</v>
       </c>
@@ -26873,7 +26879,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="428" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A428">
         <v>360146</v>
       </c>
@@ -26926,7 +26932,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="429" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A429">
         <v>492657</v>
       </c>
@@ -26979,7 +26985,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="430" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A430">
         <v>393814</v>
       </c>
@@ -27032,7 +27038,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="431" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A431">
         <v>443544</v>
       </c>
@@ -27085,7 +27091,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="432" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A432">
         <v>1082171</v>
       </c>
@@ -27138,7 +27144,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="433" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A433">
         <v>876280</v>
       </c>
@@ -27191,7 +27197,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="434" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A434">
         <v>446816</v>
       </c>
@@ -27244,7 +27250,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="435" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A435">
         <v>653742</v>
       </c>
@@ -27297,7 +27303,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="436" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A436">
         <v>435830</v>
       </c>
@@ -27350,7 +27356,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="437" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A437">
         <v>155253</v>
       </c>
@@ -27403,7 +27409,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="438" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A438">
         <v>266642</v>
       </c>
@@ -27456,7 +27462,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="439" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A439">
         <v>649132</v>
       </c>
@@ -27509,7 +27515,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="440" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A440">
         <v>604537</v>
       </c>
@@ -27562,7 +27568,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="441" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A441">
         <v>32827</v>
       </c>
@@ -27615,7 +27621,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="442" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A442">
         <v>677916</v>
       </c>
@@ -27668,7 +27674,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="443" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A443">
         <v>898615</v>
       </c>
@@ -27721,7 +27727,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="444" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A444">
         <v>842900</v>
       </c>
@@ -27774,7 +27780,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="445" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A445">
         <v>546455</v>
       </c>
@@ -27827,7 +27833,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="446" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A446">
         <v>385445</v>
       </c>
@@ -27880,7 +27886,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="447" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A447">
         <v>58067</v>
       </c>
@@ -27933,7 +27939,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="448" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A448">
         <v>311182</v>
       </c>
@@ -27986,7 +27992,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="449" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A449">
         <v>951063</v>
       </c>
@@ -28039,7 +28045,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="450" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A450">
         <v>883891</v>
       </c>
@@ -28092,7 +28098,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="451" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A451">
         <v>486028</v>
       </c>
@@ -28145,7 +28151,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="452" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A452">
         <v>583761</v>
       </c>
@@ -28198,7 +28204,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="453" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A453">
         <v>1000748</v>
       </c>
@@ -28251,7 +28257,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="454" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A454">
         <v>577898</v>
       </c>
@@ -28304,7 +28310,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="455" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A455">
         <v>1015203</v>
       </c>
@@ -28357,7 +28363,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="456" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A456">
         <v>940262</v>
       </c>
@@ -28410,7 +28416,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="457" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A457">
         <v>1144114</v>
       </c>
@@ -28463,7 +28469,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="458" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A458">
         <v>357141</v>
       </c>
@@ -28516,7 +28522,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="459" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A459">
         <v>729123</v>
       </c>
@@ -28569,7 +28575,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="460" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A460">
         <v>1000521</v>
       </c>
@@ -28622,7 +28628,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="461" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A461">
         <v>944884</v>
       </c>
@@ -28675,7 +28681,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="462" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A462">
         <v>120246</v>
       </c>
@@ -28728,7 +28734,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="463" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A463">
         <v>32720</v>
       </c>
@@ -28781,7 +28787,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="464" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A464">
         <v>1018476</v>
       </c>
@@ -28834,7 +28840,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="465" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A465">
         <v>960515</v>
       </c>
@@ -28887,7 +28893,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="466" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A466">
         <v>735147</v>
       </c>
@@ -28940,7 +28946,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="467" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A467">
         <v>186488</v>
       </c>
@@ -28993,7 +28999,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="468" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A468">
         <v>137042</v>
       </c>
@@ -29046,7 +29052,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="469" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A469">
         <v>209603</v>
       </c>
@@ -29099,7 +29105,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="470" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A470">
         <v>589469</v>
       </c>
@@ -29152,7 +29158,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="471" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A471">
         <v>471621</v>
       </c>
@@ -29205,7 +29211,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="472" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A472">
         <v>320295</v>
       </c>
@@ -29258,7 +29264,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="473" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A473">
         <v>467231</v>
       </c>
@@ -29311,7 +29317,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="474" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A474">
         <v>1087808</v>
       </c>
@@ -29364,7 +29370,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="475" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A475">
         <v>401509</v>
       </c>
@@ -29417,7 +29423,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="476" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A476">
         <v>1091760</v>
       </c>
@@ -29470,7 +29476,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="477" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A477">
         <v>629781</v>
       </c>
@@ -29523,7 +29529,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="478" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:17" ht="124" x14ac:dyDescent="0.35">
       <c r="A478">
         <v>505437</v>
       </c>
@@ -29576,7 +29582,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="479" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A479">
         <v>1058471</v>
       </c>
@@ -29629,7 +29635,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="480" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A480">
         <v>1130697</v>
       </c>
@@ -29682,7 +29688,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="481" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A481">
         <v>602154</v>
       </c>
@@ -29735,7 +29741,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="482" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A482">
         <v>408107</v>
       </c>
@@ -29788,7 +29794,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="483" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A483">
         <v>316836</v>
       </c>
@@ -29841,7 +29847,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="484" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A484">
         <v>549074</v>
       </c>
@@ -29894,7 +29900,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="485" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A485">
         <v>1084898</v>
       </c>
@@ -29947,7 +29953,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="486" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A486">
         <v>306407</v>
       </c>
@@ -30000,7 +30006,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="487" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A487">
         <v>259898</v>
       </c>
@@ -30053,7 +30059,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="488" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A488">
         <v>66645</v>
       </c>
@@ -30106,7 +30112,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="489" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A489">
         <v>155219</v>
       </c>
@@ -30159,7 +30165,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="490" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A490">
         <v>673273</v>
       </c>
@@ -30212,7 +30218,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="491" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A491">
         <v>389350</v>
       </c>
@@ -30265,7 +30271,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="492" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A492">
         <v>909900</v>
       </c>
@@ -30318,7 +30324,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="493" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A493">
         <v>836598</v>
       </c>
@@ -30371,7 +30377,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="494" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A494">
         <v>1060154</v>
       </c>
@@ -30424,7 +30430,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="495" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A495">
         <v>1100770</v>
       </c>
@@ -30477,7 +30483,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="496" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A496">
         <v>311712</v>
       </c>
@@ -30530,7 +30536,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="497" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A497">
         <v>584663</v>
       </c>
@@ -30583,7 +30589,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="498" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A498">
         <v>74028</v>
       </c>
@@ -30636,7 +30642,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="499" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:17" ht="62" x14ac:dyDescent="0.35">
       <c r="A499">
         <v>872957</v>
       </c>
@@ -30689,7 +30695,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="500" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A500">
         <v>19811</v>
       </c>
@@ -30742,7 +30748,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="501" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A501">
         <v>257034</v>
       </c>

</xml_diff>